<commit_message>
added data related to india fg and amazon cloud PMR experiments
git-svn-id: file://localhost/tmp/svn2git/svn@7787 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccpe-cloud12/performance/pmr_clouds.xlsx
+++ b/papers/ccpe-cloud12/performance/pmr_clouds.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="grid-cloud interoperability" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Number of chunks</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,18 +66,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Intermediate data generated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.73GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.5GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -89,15 +78,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7.1GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>stdev</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>stdev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR on Grids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GS Seqal application</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>half data on FG india and half data on Amazon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amazon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intermediate data generated(in GB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intermediate data generated and moved from grid to cloud(GB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -105,12 +122,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -451,11 +462,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="506357880"/>
-        <c:axId val="506360776"/>
+        <c:axId val="532932200"/>
+        <c:axId val="532950392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="506357880"/>
+        <c:axId val="532932200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,14 +501,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506360776"/>
+        <c:crossAx val="532950392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="506360776"/>
+        <c:axId val="532950392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -533,7 +544,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="506357880"/>
+        <c:crossAx val="532932200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -914,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A6:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -923,7 +934,7 @@
     <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:9" ht="39">
+    <row r="6" spans="1:9" ht="52">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -943,10 +954,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
         <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -968,8 +979,9 @@
       <c r="F7">
         <v>230.33</v>
       </c>
-      <c r="G7" t="s">
-        <v>12</v>
+      <c r="G7">
+        <f>1.73/2</f>
+        <v>0.86499999999999999</v>
       </c>
       <c r="H7">
         <f>D7+E7+F7</f>
@@ -1000,7 +1012,7 @@
         <v>1657.98</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1046,8 +1058,9 @@
       <c r="F11">
         <v>298.01</v>
       </c>
-      <c r="G11" t="s">
-        <v>13</v>
+      <c r="G11">
+        <f>3.5/2</f>
+        <v>1.75</v>
       </c>
       <c r="H11">
         <f>D11+E11+F11</f>
@@ -1078,7 +1091,7 @@
         <v>1991.6599999999999</v>
       </c>
       <c r="I12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1124,8 +1137,9 @@
       <c r="F16">
         <v>568.41</v>
       </c>
-      <c r="G16" t="s">
-        <v>17</v>
+      <c r="G16">
+        <f>7.1/2</f>
+        <v>3.55</v>
       </c>
       <c r="H16">
         <f>D16+E16+F16</f>
@@ -1191,7 +1205,7 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
@@ -1262,13 +1276,13 @@
     </row>
     <row r="29" spans="1:8">
       <c r="D29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1325,7 +1339,6 @@
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -1333,4 +1346,252 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A4:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="78">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>309.25</v>
+      </c>
+      <c r="C12">
+        <v>431.03</v>
+      </c>
+      <c r="D12">
+        <v>1395.22</v>
+      </c>
+      <c r="E12">
+        <v>33.28</v>
+      </c>
+      <c r="F12">
+        <v>292.16000000000003</v>
+      </c>
+      <c r="G12">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="H12">
+        <v>2558.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>194.97</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1491.51</v>
+      </c>
+      <c r="E13">
+        <v>39.58</v>
+      </c>
+      <c r="F13">
+        <v>344.84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>186.65</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1478.67</v>
+      </c>
+      <c r="E14">
+        <v>37.35</v>
+      </c>
+      <c r="F14">
+        <v>345.43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>484.86</v>
+      </c>
+      <c r="C16">
+        <v>523.5</v>
+      </c>
+      <c r="D16">
+        <v>1625.25</v>
+      </c>
+      <c r="E16">
+        <v>48.26</v>
+      </c>
+      <c r="F16">
+        <v>519.29999999999995</v>
+      </c>
+      <c r="G16">
+        <f>3.5/2</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>1636.66</v>
+      </c>
+      <c r="E17">
+        <v>50.44</v>
+      </c>
+      <c r="F17">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>1696.67</v>
+      </c>
+      <c r="E18">
+        <v>52.34</v>
+      </c>
+      <c r="F18">
+        <v>532.86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>780</v>
+      </c>
+      <c r="C20">
+        <v>1021.79</v>
+      </c>
+      <c r="D20">
+        <v>2760.52</v>
+      </c>
+      <c r="E20">
+        <v>95.48</v>
+      </c>
+      <c r="F20">
+        <v>962.32</v>
+      </c>
+      <c r="G20">
+        <f>7.1/2</f>
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>183.33</v>
+      </c>
+      <c r="D21">
+        <v>3167.85</v>
+      </c>
+      <c r="E21">
+        <v>92.32</v>
+      </c>
+      <c r="F21">
+        <v>843.57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>195.35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22">
+        <v>2987.6</v>
+      </c>
+      <c r="E22">
+        <v>98.34</v>
+      </c>
+      <c r="F22">
+        <v>896.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>